<commit_message>
feat: Correção das planilhas
</commit_message>
<xml_diff>
--- a/src/main/resources/planilhas/Curso_EngenhariaMecanica_Matutino.xlsx
+++ b/src/main/resources/planilhas/Curso_EngenhariaMecanica_Matutino.xlsx
@@ -627,7 +627,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -651,7 +651,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
-    <font/>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -681,7 +680,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -708,34 +707,18 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -744,18 +727,31 @@
     <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -978,793 +974,625 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
+      <c r="G2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>1.0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8">
+      <c r="C3" s="9">
         <v>2.0</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="8">
+      <c r="D3" s="9">
         <v>80.0</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="7" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
+      <c r="G3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4">
-      <c r="A4" s="6">
+      <c r="A4" s="7">
         <v>2.0</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="8">
+      <c r="C4" s="9">
         <v>2.0</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="8">
+      <c r="D4" s="9">
         <v>80.0</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="7" t="s">
+      <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4"/>
+      <c r="G4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5">
-      <c r="A5" s="6">
+      <c r="A5" s="7">
         <v>3.0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="8">
+      <c r="C5" s="9">
         <v>2.0</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="8">
+      <c r="D5" s="9">
         <v>80.0</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4"/>
+      <c r="G5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6">
-      <c r="A6" s="6">
+      <c r="A6" s="7">
         <v>4.0</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8">
+      <c r="C6" s="9">
         <v>2.0</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="8">
+      <c r="D6" s="9">
         <v>40.0</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="7" t="s">
+      <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="4"/>
+      <c r="G6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7">
-      <c r="A7" s="6">
+      <c r="A7" s="7">
         <v>5.0</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8">
+      <c r="C7" s="9">
         <v>2.0</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="8">
+      <c r="D7" s="9">
         <v>80.0</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="7" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="4"/>
+      <c r="G7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8">
-      <c r="A8" s="6">
+      <c r="A8" s="7">
         <v>6.0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="8">
+      <c r="C8" s="9">
         <v>2.0</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8">
+      <c r="D8" s="9">
         <v>40.0</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="7" t="s">
+      <c r="E8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="4"/>
+      <c r="G8" s="11"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>7.0</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="8">
+      <c r="C9" s="9">
         <v>4.0</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="8">
+      <c r="D9" s="9">
         <v>80.0</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="7" t="s">
+      <c r="E9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="4"/>
+      <c r="G9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>8.0</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="8">
+      <c r="C10" s="9">
         <v>4.0</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="8">
+      <c r="D10" s="9">
         <v>80.0</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="7" t="s">
+      <c r="E10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
+      <c r="G10" s="11"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>9.0</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="8">
+      <c r="C11" s="9">
         <v>4.0</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="8">
+      <c r="D11" s="9">
         <v>80.0</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="7" t="s">
+      <c r="E11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="4"/>
+      <c r="G11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12">
-      <c r="A12" s="6">
+      <c r="A12" s="7">
         <v>10.0</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="8">
+      <c r="C12" s="9">
         <v>4.0</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="8">
+      <c r="D12" s="9">
         <v>80.0</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="7" t="s">
+      <c r="E12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="4"/>
+      <c r="G12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13">
-      <c r="A13" s="6">
+      <c r="A13" s="7">
         <v>11.0</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="8">
+      <c r="C13" s="9">
         <v>4.0</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="8">
+      <c r="D13" s="9">
         <v>40.0</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="7" t="s">
+      <c r="E13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="4"/>
+      <c r="G13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>12.0</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="8">
+      <c r="C14" s="9">
         <v>4.0</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="8">
+      <c r="D14" s="9">
         <v>40.0</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="7" t="s">
+      <c r="E14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="4"/>
+      <c r="G14" s="11"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15">
-      <c r="A15" s="6">
+      <c r="A15" s="7">
         <v>13.0</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="8">
+      <c r="C15" s="9">
         <v>6.0</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="8">
+      <c r="D15" s="9">
         <v>80.0</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="7" t="s">
+      <c r="E15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="4"/>
+      <c r="G15" s="11"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16">
-      <c r="A16" s="6">
+      <c r="A16" s="7">
         <v>14.0</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="8">
+      <c r="C16" s="9">
         <v>6.0</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="8">
+      <c r="D16" s="9">
         <v>80.0</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="7" t="s">
+      <c r="E16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="4"/>
+      <c r="G16" s="11"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="6">
+      <c r="A17" s="7">
         <v>15.0</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="8">
+      <c r="C17" s="9">
         <v>6.0</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="8">
+      <c r="D17" s="9">
         <v>80.0</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="7" t="s">
+      <c r="E17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="4"/>
+      <c r="G17" s="11"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
     </row>
     <row r="18">
-      <c r="A18" s="2">
+      <c r="A18" s="3">
         <v>16.0</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="8">
+      <c r="C18" s="9">
         <v>6.0</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="8">
+      <c r="D18" s="9">
         <v>40.0</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="7" t="s">
+      <c r="E18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="4"/>
+      <c r="G18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
     </row>
     <row r="19">
-      <c r="A19" s="2">
+      <c r="A19" s="3">
         <v>17.0</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="8">
+      <c r="C19" s="9">
         <v>6.0</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="8">
+      <c r="D19" s="9">
         <v>40.0</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="7" t="s">
+      <c r="E19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="4"/>
+      <c r="G19" s="11"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
     </row>
     <row r="20">
-      <c r="A20" s="2">
+      <c r="A20" s="3">
         <v>18.0</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="8">
+      <c r="C20" s="9">
         <v>6.0</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="8">
+      <c r="D20" s="9">
         <v>80.0</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="7" t="s">
+      <c r="E20" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="4"/>
+      <c r="G20" s="11"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21">
-      <c r="A21" s="6">
+      <c r="A21" s="7">
         <v>19.0</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="8">
+      <c r="C21" s="9">
         <v>8.0</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="8">
+      <c r="D21" s="9">
         <v>80.0</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="7" t="s">
+      <c r="E21" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="4"/>
+      <c r="G21" s="11"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="22">
-      <c r="A22" s="6">
+      <c r="A22" s="7">
         <v>20.0</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="8">
+      <c r="C22" s="9">
         <v>8.0</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="8">
+      <c r="D22" s="9">
         <v>40.0</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="7" t="s">
+      <c r="E22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="4"/>
+      <c r="G22" s="11"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
     </row>
     <row r="23">
-      <c r="A23" s="6">
+      <c r="A23" s="7">
         <v>21.0</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="8">
+      <c r="C23" s="9">
         <v>8.0</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="8">
+      <c r="D23" s="9">
         <v>40.0</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="7" t="s">
+      <c r="E23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="4"/>
+      <c r="G23" s="11"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
     </row>
     <row r="24">
-      <c r="A24" s="9">
+      <c r="A24" s="13">
         <v>22.0</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="8">
+      <c r="C24" s="9">
         <v>8.0</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="8">
+      <c r="D24" s="9">
         <v>40.0</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="7" t="s">
+      <c r="E24" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="4"/>
+      <c r="G24" s="11"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
     </row>
     <row r="25">
-      <c r="A25" s="9">
+      <c r="A25" s="13">
         <v>23.0</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="8">
+      <c r="C25" s="9">
         <v>8.0</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="8">
+      <c r="D25" s="9">
         <v>40.0</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="7" t="s">
+      <c r="E25" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="4"/>
+      <c r="G25" s="11"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26">
-      <c r="A26" s="9">
+      <c r="A26" s="13">
         <v>24.0</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="8">
+      <c r="C26" s="9">
         <v>8.0</v>
       </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="8">
+      <c r="D26" s="9">
         <v>40.0</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="7" t="s">
+      <c r="E26" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="4"/>
+      <c r="G26" s="11"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
     </row>
     <row r="27">
-      <c r="A27" s="9">
+      <c r="A27" s="13">
         <v>25.0</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="8">
+      <c r="C27" s="9">
         <v>8.0</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="8">
+      <c r="D27" s="9">
         <v>40.0</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="7" t="s">
+      <c r="E27" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="4"/>
+      <c r="G27" s="11"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28">
-      <c r="A28" s="9">
+      <c r="A28" s="13">
         <v>26.0</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="8">
+      <c r="C28" s="9">
         <v>8.0</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="8">
+      <c r="D28" s="9">
         <v>80.0</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="7" t="s">
+      <c r="E28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="4"/>
+      <c r="G28" s="11"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29">
-      <c r="A29" s="9">
+      <c r="A29" s="13">
         <v>27.0</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="8">
+      <c r="C29" s="9">
         <v>10.0</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="8">
+      <c r="D29" s="9">
         <v>80.0</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="7" t="s">
+      <c r="E29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="4"/>
+      <c r="G29" s="11"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
     </row>
     <row r="30">
-      <c r="A30" s="9">
+      <c r="A30" s="13">
         <v>28.0</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="8">
+      <c r="C30" s="9">
         <v>10.0</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="8">
+      <c r="D30" s="9">
         <v>80.0</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="7" t="s">
+      <c r="E30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="4"/>
+      <c r="G30" s="11"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="117">
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Adição planilha disponibilidade dos professores
</commit_message>
<xml_diff>
--- a/src/main/resources/planilhas/Curso_EngenhariaMecanica_Matutino.xlsx
+++ b/src/main/resources/planilhas/Curso_EngenhariaMecanica_Matutino.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Curso: Engenharia Mecânica (Matutino)</t>
   </si>
@@ -580,46 +580,6 @@
         <sz val="11.0"/>
       </rPr>
       <t>Natalia Madalena Boelter</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Trabalho de Conclusão de Curso II</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Matheus Fontanelle Pereira</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Atividades de Extensão V</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <color theme="1"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t>Fernando da Silva Osório</t>
     </r>
   </si>
 </sst>
@@ -711,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -752,6 +712,12 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1531,13 +1497,13 @@
       <c r="A28" s="13">
         <v>26.0</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="14">
         <v>8.0</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="14">
         <v>80.0</v>
       </c>
       <c r="E28" s="10" t="s">
@@ -1549,42 +1515,22 @@
       <c r="K28" s="12"/>
     </row>
     <row r="29">
-      <c r="A29" s="13">
-        <v>27.0</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="D29" s="9">
-        <v>80.0</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>59</v>
-      </c>
+      <c r="A29" s="15"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
       <c r="G29" s="11"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
     </row>
     <row r="30">
-      <c r="A30" s="13">
-        <v>28.0</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="D30" s="9">
-        <v>80.0</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="A30" s="15"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
       <c r="G30" s="11"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>

</xml_diff>